<commit_message>
Add group, imei, model, sim number to summary
</commit_message>
<xml_diff>
--- a/templates/export/summary.xlsx
+++ b/templates/export/summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/srihariayapilla/Documents/Office/traccar/templates/export/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sainathavadhuta/Documents/code/traccar/templates/export/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36D9DEC-F2BF-2A4E-9EC4-41F97189D1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09FDCC7-361F-F045-BE35-65C6D9CCDA3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="G7")</t>
+          <t>jx:area(lastCell="K7")</t>
         </r>
       </text>
     </comment>
@@ -54,7 +54,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="summaries", var="summary", lastCell="G7")</t>
+          <t>jx:each(items="summaries", var="summary", lastCell="K7")</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Report type:</t>
   </si>
@@ -111,6 +111,30 @@
   </si>
   <si>
     <t>${volumeUnit.equals("impGal") ? "".format("%.1f Imp. Gal", summary.spentFuel / 4.546) : volumeUnit.equals("usGal") ? "".format("%.1f U.S. Gal", summary.spentFuel / 3.785) : "".format("%.1f l", summary.spentFuel)}</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>${summary.groupName}</t>
+  </si>
+  <si>
+    <t>IMEI</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>SIM Number</t>
+  </si>
+  <si>
+    <t>${summary.imei}</t>
+  </si>
+  <si>
+    <t>${summary.model}</t>
+  </si>
+  <si>
+    <t>${summary.phone}</t>
   </si>
 </sst>
 </file>
@@ -685,6 +709,114 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EBB3C1B5-1D91-5392-4890-63A524B3C148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B5C761AC-5A52-1462-4076-B36BA81D7CD5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -985,26 +1117,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="29" width="8.6640625" customWidth="1"/>
+    <col min="5" max="7" width="16.33203125" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" customWidth="1"/>
+    <col min="9" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.6640625" customWidth="1"/>
+    <col min="12" max="29" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
       <c r="E1" s="5"/>
     </row>
-    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1014,13 +1149,13 @@
       <c r="C2" s="6"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1031,7 +1166,7 @@
       <c r="E4" s="5"/>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1042,7 +1177,7 @@
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
     </row>
-    <row r="6" spans="1:9" s="11" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" s="11" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>4</v>
       </c>
@@ -1062,8 +1197,20 @@
       <c r="G6" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>10</v>
       </c>
@@ -1082,6 +1229,18 @@
       </c>
       <c r="G7" s="14" t="s">
         <v>15</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactor: Rename 'IMEI' to 'Unique ID' in Summary Report
- Updated `SummaryReportProvider` to use `UniqueId` instead of `Imei` for consistency.
- Renamed `imei` to `uniqueId` in `SummaryReportItem` model.
- Adjusted corresponding getter and setter methods.
- Updated the export template (`summary.xlsx`) to reflect the new column header.
</commit_message>
<xml_diff>
--- a/templates/export/summary.xlsx
+++ b/templates/export/summary.xlsx
@@ -112,7 +112,7 @@
     <t>${summary.groupName}</t>
   </si>
   <si>
-    <t>${summary.imei}</t>
+    <t>${summary.uniqueId}</t>
   </si>
   <si>
     <t>${summary.model}</t>
@@ -292,31 +292,31 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="3" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -331,7 +331,7 @@
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -558,17 +558,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -595,10 +595,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -837,12 +837,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1119,7 +1119,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1146,10 +1146,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>